<commit_message>
added prefixes sheet and referenced its csv in script
by moving the prefixes table from resources folder to the spreadsheet we improve users input to it
</commit_message>
<xml_diff>
--- a/test/test-input.xlsx
+++ b/test/test-input.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5810267A-EE9F-4289-A545-D3AF67CAE707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52AEAD5-BA2F-4305-83D1-20E666A6D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -16,8 +16,9 @@
     <sheet name="IndAttributes" sheetId="6" r:id="rId6"/>
     <sheet name="Datatypes" sheetId="7" r:id="rId7"/>
     <sheet name="UpperClasses" sheetId="8" r:id="rId8"/>
-    <sheet name="OntologyMetadata" sheetId="9" r:id="rId9"/>
-    <sheet name="README" sheetId="10" r:id="rId10"/>
+    <sheet name="prefixes" sheetId="11" r:id="rId9"/>
+    <sheet name="OntologyMetadata" sheetId="9" r:id="rId10"/>
+    <sheet name="README" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Attributes!$A$1:$G$3</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>Domain</t>
   </si>
@@ -260,6 +261,51 @@
   </si>
   <si>
     <t>Test Input Version 1</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>iri</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/elements/1.1/</t>
+  </si>
+  <si>
+    <t>owl</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2002/07/owl#</t>
+  </si>
+  <si>
+    <t>xsd</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2001/XMLSchema#</t>
+  </si>
+  <si>
+    <t>emmo</t>
+  </si>
+  <si>
+    <t>http://emmo.info/emmo#</t>
+  </si>
+  <si>
+    <t>pmdco</t>
+  </si>
+  <si>
+    <t>https://material-digital.de/pmdco/</t>
+  </si>
+  <si>
+    <t>spo</t>
+  </si>
+  <si>
+    <t>https://w3id.org/steel/ProcessOntology/</t>
+  </si>
+  <si>
+    <t>base</t>
   </si>
 </sst>
 </file>
@@ -471,29 +517,7 @@
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1343,10 +1367,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B90:B1048576 B1:B88">
-    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="duplicateValues" dxfId="23" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1354,6 +1378,49 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="21.75" bestFit="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="18" customFormat="1" ht="18.75">
+      <c r="A1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:D10"/>
   <sheetViews>
@@ -1534,10 +1601,10 @@
   </sheetData>
   <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576 F1:F1048576 G3">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1703,10 +1770,10 @@
   </sheetData>
   <autoFilter ref="A1:G3" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4 B13 E1:E1048576 B22:B1048576 F3">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1775,10 +1842,10 @@
   </sheetData>
   <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576 D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1831,10 +1898,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157500000008" bottom="0.78740157500000008" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
@@ -1866,9 +1933,7 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
@@ -1906,10 +1971,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157500000008" bottom="0.78740157500000008" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
@@ -2252,34 +2317,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A2 A4:A9 A11 A13:A30 A33:A41 A43:A48 A51:A58 A60:A82">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A42">
-    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="duplicateValues" dxfId="2" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50">
-    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59">
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
   </conditionalFormatting>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
@@ -2287,44 +2352,86 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8A85308-2C47-4318-9DC9-6D6600842E8A}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.75" bestFit="1"/>
-    <col min="2" max="2" width="23.625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1"/>
+    <col min="2" max="2" width="34.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="18" customFormat="1" ht="18.75">
-      <c r="A1" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    <row r="1" spans="1:2" ht="18.75">
+      <c r="A1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated test to include a prefix reference as well
</commit_message>
<xml_diff>
--- a/test/test-input.xlsx
+++ b/test/test-input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52AEAD5-BA2F-4305-83D1-20E666A6D527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48B94ED-96F1-4509-8734-DB8DB491E15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
   <si>
     <t>Domain</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>owl:Class</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -472,13 +475,12 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1000,11 +1002,11 @@
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F7" sqref="F7"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
@@ -1050,319 +1052,319 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="10" customFormat="1">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:10" customFormat="1">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:10" customFormat="1">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="10" customFormat="1">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:10" customFormat="1">
+      <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="10" customFormat="1">
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" customFormat="1">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:10" s="10" customFormat="1">
+    <row r="6" spans="1:10" customFormat="1">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1">
+    <row r="7" spans="1:10" customFormat="1">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:10" s="10" customFormat="1">
+    <row r="8" spans="1:10" customFormat="1">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:10" s="10" customFormat="1">
+    <row r="9" spans="1:10" customFormat="1">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:10" s="10" customFormat="1">
+    <row r="10" spans="1:10" customFormat="1">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:10" s="10" customFormat="1">
+    <row r="11" spans="1:10" customFormat="1">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:10" s="10" customFormat="1">
+    <row r="12" spans="1:10" customFormat="1">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:10" s="10" customFormat="1">
+    <row r="13" spans="1:10" customFormat="1">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:10" s="10" customFormat="1">
+    <row r="14" spans="1:10" customFormat="1">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:10" s="10" customFormat="1">
+    <row r="15" spans="1:10" customFormat="1">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:10" s="10" customFormat="1">
+    <row r="16" spans="1:10" customFormat="1">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" s="10" customFormat="1">
+    <row r="17" spans="2:2" customFormat="1">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" s="10" customFormat="1">
+    <row r="18" spans="2:2" customFormat="1">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" s="10" customFormat="1">
+    <row r="19" spans="2:2" customFormat="1">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" s="10" customFormat="1">
+    <row r="20" spans="2:2" customFormat="1">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" s="10" customFormat="1">
+    <row r="21" spans="2:2" customFormat="1">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" s="10" customFormat="1">
+    <row r="22" spans="2:2" customFormat="1">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" s="10" customFormat="1">
+    <row r="23" spans="2:2" customFormat="1">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" s="10" customFormat="1">
+    <row r="24" spans="2:2" customFormat="1">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:2" s="10" customFormat="1">
+    <row r="25" spans="2:2" customFormat="1">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:2" s="10" customFormat="1">
+    <row r="26" spans="2:2" customFormat="1">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="2:2" s="10" customFormat="1">
+    <row r="27" spans="2:2" customFormat="1">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="2:2" s="10" customFormat="1">
+    <row r="28" spans="2:2" customFormat="1">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="2:2" s="10" customFormat="1">
+    <row r="29" spans="2:2" customFormat="1">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" s="10" customFormat="1">
+    <row r="30" spans="2:2" customFormat="1">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" s="10" customFormat="1">
+    <row r="31" spans="2:2" customFormat="1">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" s="10" customFormat="1">
+    <row r="32" spans="2:2" customFormat="1">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" s="10" customFormat="1">
+    <row r="33" spans="2:2" customFormat="1">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" s="10" customFormat="1">
+    <row r="34" spans="2:2" customFormat="1">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" s="10" customFormat="1">
+    <row r="35" spans="2:2" customFormat="1">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" s="10" customFormat="1">
+    <row r="36" spans="2:2" customFormat="1">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" s="10" customFormat="1">
+    <row r="37" spans="2:2" customFormat="1">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" s="10" customFormat="1">
+    <row r="38" spans="2:2" customFormat="1">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" s="10" customFormat="1">
+    <row r="39" spans="2:2" customFormat="1">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" s="10" customFormat="1">
+    <row r="40" spans="2:2" customFormat="1">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" s="10" customFormat="1">
+    <row r="41" spans="2:2" customFormat="1">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" s="10" customFormat="1">
+    <row r="42" spans="2:2" customFormat="1">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" s="10" customFormat="1">
+    <row r="43" spans="2:2" customFormat="1">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" s="10" customFormat="1">
+    <row r="44" spans="2:2" customFormat="1">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" s="10" customFormat="1">
+    <row r="45" spans="2:2" customFormat="1">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" s="10" customFormat="1">
+    <row r="46" spans="2:2" customFormat="1">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" s="10" customFormat="1">
+    <row r="47" spans="2:2" customFormat="1">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" s="10" customFormat="1">
+    <row r="48" spans="2:2" customFormat="1">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="2:2" s="10" customFormat="1">
+    <row r="49" spans="2:2" customFormat="1">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="2:2" s="10" customFormat="1">
+    <row r="50" spans="2:2" customFormat="1">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="2:2" s="10" customFormat="1">
+    <row r="51" spans="2:2" customFormat="1">
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="2:2" s="10" customFormat="1">
+    <row r="52" spans="2:2" customFormat="1">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="2:2" s="10" customFormat="1">
+    <row r="53" spans="2:2" customFormat="1">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="2:2" s="10" customFormat="1">
+    <row r="54" spans="2:2" customFormat="1">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="2:2" s="10" customFormat="1">
+    <row r="55" spans="2:2" customFormat="1">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="2:2" s="10" customFormat="1">
+    <row r="56" spans="2:2" customFormat="1">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="2:2" s="10" customFormat="1">
+    <row r="57" spans="2:2" customFormat="1">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="2:2" s="10" customFormat="1">
+    <row r="58" spans="2:2" customFormat="1">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="2:2" s="10" customFormat="1">
+    <row r="59" spans="2:2" customFormat="1">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="2:2" s="10" customFormat="1">
+    <row r="60" spans="2:2" customFormat="1">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="2:2" s="10" customFormat="1">
+    <row r="61" spans="2:2" customFormat="1">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="2:2" s="10" customFormat="1">
+    <row r="62" spans="2:2" customFormat="1">
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="2:2" s="10" customFormat="1">
+    <row r="63" spans="2:2" customFormat="1">
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="2:2" s="10" customFormat="1">
+    <row r="64" spans="2:2" customFormat="1">
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="2:2" s="10" customFormat="1">
+    <row r="65" spans="2:2" customFormat="1">
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="2:2" s="10" customFormat="1">
+    <row r="66" spans="2:2" customFormat="1">
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="2:2" s="10" customFormat="1">
+    <row r="67" spans="2:2" customFormat="1">
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="2:2" s="10" customFormat="1">
+    <row r="68" spans="2:2" customFormat="1">
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="2:2" s="10" customFormat="1">
+    <row r="69" spans="2:2" customFormat="1">
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="2:2" s="10" customFormat="1">
+    <row r="70" spans="2:2" customFormat="1">
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="2:2" s="10" customFormat="1">
+    <row r="71" spans="2:2" customFormat="1">
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="2:2" s="10" customFormat="1">
+    <row r="72" spans="2:2" customFormat="1">
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="2:2" s="10" customFormat="1">
+    <row r="73" spans="2:2" customFormat="1">
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="2:2" s="10" customFormat="1">
+    <row r="74" spans="2:2" customFormat="1">
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="2:2" s="10" customFormat="1">
+    <row r="75" spans="2:2" customFormat="1">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="2:2" s="10" customFormat="1">
+    <row r="76" spans="2:2" customFormat="1">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="2:2" s="10" customFormat="1">
+    <row r="77" spans="2:2" customFormat="1">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="2:2" s="10" customFormat="1">
+    <row r="78" spans="2:2" customFormat="1">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="2:2" s="10" customFormat="1">
+    <row r="79" spans="2:2" customFormat="1">
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="2:2" s="10" customFormat="1">
+    <row r="80" spans="2:2" customFormat="1">
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="2:2" s="10" customFormat="1">
+    <row r="81" spans="2:2" customFormat="1">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2" s="10" customFormat="1">
+    <row r="82" spans="2:2" customFormat="1">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2" s="10" customFormat="1">
+    <row r="83" spans="2:2" customFormat="1">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2" s="10" customFormat="1">
+    <row r="84" spans="2:2" customFormat="1">
       <c r="B84" s="2"/>
     </row>
   </sheetData>
@@ -1392,14 +1394,14 @@
     <col min="3" max="3" width="16.5" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="18" customFormat="1" ht="18.75">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:3" s="17" customFormat="1" ht="18.75">
+      <c r="A1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1430,60 +1432,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="10" style="20" customWidth="1"/>
+    <col min="1" max="1" width="25.875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="10" style="19" customWidth="1"/>
     <col min="3" max="3" width="106.625" customWidth="1"/>
     <col min="4" max="4" width="11.625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="23.25">
-      <c r="A2" s="21"/>
-      <c r="C2" s="22"/>
+      <c r="A2" s="20"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:4" ht="23.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="24"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" ht="23.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="24"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" ht="23.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="24"/>
-    </row>
-    <row r="6" spans="1:4" s="26" customFormat="1">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:4" s="25" customFormat="1">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="24"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="24"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="24"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="C10" s="29"/>
+      <c r="C10" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1550,19 +1552,19 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1570,25 +1572,25 @@
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
       <c r="G3" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="12"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
@@ -1628,7 +1630,7 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1640,7 +1642,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="12" customWidth="1"/>
     <col min="2" max="2" width="25.875" customWidth="1"/>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="4" max="4" width="17.625" customWidth="1"/>
@@ -1673,7 +1675,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
@@ -1688,84 +1690,60 @@
       <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" t="s">
         <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="C10" s="10"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="C12" s="10"/>
-    </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="14"/>
+      <c r="B42" s="13"/>
     </row>
     <row r="43" spans="2:2">
-      <c r="B43" s="14"/>
+      <c r="B43" s="13"/>
     </row>
     <row r="44" spans="2:2">
-      <c r="B44" s="14"/>
+      <c r="B44" s="13"/>
     </row>
     <row r="45" spans="2:2">
-      <c r="B45" s="14"/>
+      <c r="B45" s="13"/>
     </row>
     <row r="46" spans="2:2">
-      <c r="B46" s="14"/>
+      <c r="B46" s="13"/>
     </row>
     <row r="47" spans="2:2">
-      <c r="B47" s="14"/>
+      <c r="B47" s="13"/>
     </row>
     <row r="48" spans="2:2">
-      <c r="B48" s="14"/>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="14"/>
-    </row>
-    <row r="51" spans="2:3">
-      <c r="C51" s="10"/>
+      <c r="B48" s="13"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G3" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
@@ -1815,7 +1793,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="15" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="14" customWidth="1"/>
     <col min="2" max="2" width="25.875" customWidth="1"/>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
@@ -1897,11 +1875,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157500000008" bottom="0.78740157500000008" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
@@ -1959,22 +1937,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="D2" s="10"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="D3" s="10"/>
-    </row>
     <row r="4" spans="1:5">
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157500000008" bottom="0.78740157500000008" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
@@ -2025,8 +1997,8 @@
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="17" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:1" s="16" customFormat="1" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed unintended rendering of prefixed ids, updated to SeMiFuLi 0.2.1
SeMiFuLi 0.2.1 adds contains and notContains function

ommit rendering of (foreign) ids containing a colon(:)
</commit_message>
<xml_diff>
--- a/test/test-input.xlsx
+++ b/test/test-input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48B94ED-96F1-4509-8734-DB8DB491E15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33EF0C0-C51A-423C-BCC8-427DEBBB54D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="35685" windowHeight="19230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="92">
   <si>
     <t>Domain</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>owl:Class</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Klasse</t>
+  </si>
+  <si>
+    <t>OWL</t>
   </si>
 </sst>
 </file>
@@ -1002,11 +1011,11 @@
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F7" sqref="F7"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
@@ -1128,7 +1137,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" customFormat="1">
-      <c r="B5" s="2"/>
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:10" customFormat="1">
       <c r="B6" s="2"/>

</xml_diff>

<commit_message>
added more ontology metadata
</commit_message>
<xml_diff>
--- a/test/test-input.xlsx
+++ b/test/test-input.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33EF0C0-C51A-423C-BCC8-427DEBBB54D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24BBF2A-910A-4437-AA45-9876AD897769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="35685" windowHeight="19230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -41,8 +41,62 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={6A6C5CF8-F4E8-4CA8-8374-C756CE1FDA5F}</author>
+    <author>tc={704B6077-2554-483E-80B3-40238DF20705}</author>
+    <author>tc={E66E2A3F-7B19-4BB7-8DE0-C3E4C58A5B68}</author>
+    <author>tc={8C82DEC2-E0DA-4628-BD35-89B1B0EC3B02}</author>
+    <author>tc={E1ADD663-58B7-4105-8D38-8C3BDCFC6570}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{6A6C5CF8-F4E8-4CA8-8374-C756CE1FDA5F}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Suggested prefix for this ontology</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{704B6077-2554-483E-80B3-40238DF20705}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Semicolon (";") separated list of persons that should be listed as contributors</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="2" shapeId="0" xr:uid="{E66E2A3F-7B19-4BB7-8DE0-C3E4C58A5B68}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Date in ISO-Format (YYYY-MM-DD) the ontology was initially created</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="3" shapeId="0" xr:uid="{8C82DEC2-E0DA-4628-BD35-89B1B0EC3B02}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    URL to the licence for this ontology</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="4" shapeId="0" xr:uid="{E1ADD663-58B7-4105-8D38-8C3BDCFC6570}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    dcterms:rights string to add to the ontology metadata</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
   <si>
     <t>Domain</t>
   </si>
@@ -318,13 +372,49 @@
   </si>
   <si>
     <t>OWL</t>
+  </si>
+  <si>
+    <t>https://creativecommons.org/licenses/by/4.0/</t>
+  </si>
+  <si>
+    <t>CC-BY xlsx2owl</t>
+  </si>
+  <si>
+    <t>contributor</t>
+  </si>
+  <si>
+    <t>prefPrefix</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>2023-06-01</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>copyright</t>
+  </si>
+  <si>
+    <t>depiction</t>
+  </si>
+  <si>
+    <t>base:graph.png</t>
+  </si>
+  <si>
+    <t>Author 1;Author 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -385,6 +475,27 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -459,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -494,7 +605,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -523,6 +633,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -795,6 +908,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1003,6 +1120,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2024-02-15T11:16:51.68" personId="{00000000-0000-0000-0000-000000000000}" id="{6A6C5CF8-F4E8-4CA8-8374-C756CE1FDA5F}">
+    <text>Suggested prefix for this ontology</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2024-02-15T11:17:27.31" personId="{00000000-0000-0000-0000-000000000000}" id="{704B6077-2554-483E-80B3-40238DF20705}">
+    <text>Semicolon (";") separated list of persons that should be listed as contributors</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2024-02-15T11:18:11.39" personId="{00000000-0000-0000-0000-000000000000}" id="{E66E2A3F-7B19-4BB7-8DE0-C3E4C58A5B68}">
+    <text>Date in ISO-Format (YYYY-MM-DD) the ontology was initially created</text>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2024-02-15T11:18:31.51" personId="{00000000-0000-0000-0000-000000000000}" id="{8C82DEC2-E0DA-4628-BD35-89B1B0EC3B02}">
+    <text>URL to the licence for this ontology</text>
+  </threadedComment>
+  <threadedComment ref="H1" dT="2024-02-15T11:19:18.98" personId="{00000000-0000-0000-0000-000000000000}" id="{E1ADD663-58B7-4105-8D38-8C3BDCFC6570}">
+    <text>dcterms:rights string to add to the ontology metadata</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
@@ -1010,7 +1147,7 @@
   </sheetPr>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F7" sqref="F7"/>
       <selection pane="topRight"/>
@@ -1018,7 +1155,7 @@
       <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
@@ -1029,7 +1166,7 @@
     <col min="11" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" customFormat="1">
+    <row r="2" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1227,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:10" customFormat="1">
+    <row r="3" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1110,7 +1247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" customFormat="1">
+    <row r="4" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1136,7 +1273,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:10" customFormat="1">
+    <row r="5" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1150,241 +1287,241 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:10" customFormat="1">
+    <row r="6" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:10" customFormat="1">
+    <row r="7" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:10" customFormat="1">
+    <row r="8" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:10" customFormat="1">
+    <row r="9" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:10" customFormat="1">
+    <row r="10" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:10" customFormat="1">
+    <row r="11" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:10" customFormat="1">
+    <row r="12" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:10" customFormat="1">
+    <row r="13" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:10" customFormat="1">
+    <row r="14" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:10" customFormat="1">
+    <row r="15" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:10" customFormat="1">
+    <row r="16" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" customFormat="1">
+    <row r="17" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" customFormat="1">
+    <row r="18" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" customFormat="1">
+    <row r="19" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" customFormat="1">
+    <row r="20" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" customFormat="1">
+    <row r="21" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" customFormat="1">
+    <row r="22" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" customFormat="1">
+    <row r="23" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" customFormat="1">
+    <row r="24" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="2:2" customFormat="1">
+    <row r="25" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="2:2" customFormat="1">
+    <row r="26" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="2:2" customFormat="1">
+    <row r="27" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="2:2" customFormat="1">
+    <row r="28" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="2:2" customFormat="1">
+    <row r="29" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="2:2" customFormat="1">
+    <row r="30" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="2:2" customFormat="1">
+    <row r="31" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="2:2" customFormat="1">
+    <row r="32" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" customFormat="1">
+    <row r="33" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="2:2" customFormat="1">
+    <row r="34" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="2:2" customFormat="1">
+    <row r="35" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:2" customFormat="1">
+    <row r="36" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:2" customFormat="1">
+    <row r="37" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="2:2" customFormat="1">
+    <row r="38" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:2" customFormat="1">
+    <row r="39" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="2:2" customFormat="1">
+    <row r="40" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="2:2" customFormat="1">
+    <row r="41" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
     </row>
-    <row r="42" spans="2:2" customFormat="1">
+    <row r="42" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="2:2" customFormat="1">
+    <row r="43" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="2:2" customFormat="1">
+    <row r="44" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="2:2" customFormat="1">
+    <row r="45" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="2:2" customFormat="1">
+    <row r="46" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="2:2" customFormat="1">
+    <row r="47" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
     </row>
-    <row r="48" spans="2:2" customFormat="1">
+    <row r="48" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="2:2" customFormat="1">
+    <row r="49" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="2:2" customFormat="1">
+    <row r="50" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="2:2" customFormat="1">
+    <row r="51" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="2:2" customFormat="1">
+    <row r="52" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="2:2" customFormat="1">
+    <row r="53" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="2:2" customFormat="1">
+    <row r="54" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="2:2" customFormat="1">
+    <row r="55" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="2:2" customFormat="1">
+    <row r="56" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="2:2" customFormat="1">
+    <row r="57" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="2:2" customFormat="1">
+    <row r="58" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="2:2" customFormat="1">
+    <row r="59" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="2:2" customFormat="1">
+    <row r="60" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="2:2" customFormat="1">
+    <row r="61" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="2:2" customFormat="1">
+    <row r="62" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
     </row>
-    <row r="63" spans="2:2" customFormat="1">
+    <row r="63" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="2:2" customFormat="1">
+    <row r="64" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="2:2" customFormat="1">
+    <row r="65" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="2:2" customFormat="1">
+    <row r="66" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="2:2" customFormat="1">
+    <row r="67" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="2:2" customFormat="1">
+    <row r="68" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="2:2" customFormat="1">
+    <row r="69" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="2:2" customFormat="1">
+    <row r="70" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="2:2" customFormat="1">
+    <row r="71" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="2:2" customFormat="1">
+    <row r="72" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="2:2" customFormat="1">
+    <row r="73" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="2:2" customFormat="1">
+    <row r="74" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="2:2" customFormat="1">
+    <row r="75" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="2:2" customFormat="1">
+    <row r="76" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="2:2" customFormat="1">
+    <row r="77" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="2:2" customFormat="1">
+    <row r="78" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="2:2" customFormat="1">
+    <row r="79" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="2:2" customFormat="1">
+    <row r="80" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="2:2" customFormat="1">
+    <row r="81" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2" customFormat="1">
+    <row r="82" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2" customFormat="1">
+    <row r="83" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2" customFormat="1">
+    <row r="84" spans="2:2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B84" s="2"/>
     </row>
   </sheetData>
@@ -1400,32 +1537,55 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.75" bestFit="1"/>
     <col min="2" max="2" width="23.625" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1"/>
+    <col min="4" max="4" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="17" customFormat="1" ht="18.75">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1434,11 +1594,30 @@
       </c>
       <c r="C2" t="s">
         <v>72</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="2147483648" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1450,62 +1629,62 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.875" style="19" customWidth="1"/>
-    <col min="2" max="2" width="10" style="19" customWidth="1"/>
+    <col min="1" max="1" width="25.875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="10" style="18" customWidth="1"/>
     <col min="3" max="3" width="106.625" customWidth="1"/>
     <col min="4" max="4" width="11.625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="23.25">
-      <c r="A2" s="20"/>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" ht="23.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="23"/>
-    </row>
-    <row r="4" spans="1:4" ht="23.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="23"/>
-    </row>
-    <row r="5" spans="1:4" ht="23.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:4" s="25" customFormat="1">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="23"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="28"/>
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1528,7 +1707,7 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.875" style="5" customWidth="1"/>
     <col min="2" max="3" width="25.875" customWidth="1"/>
@@ -1539,7 +1718,7 @@
     <col min="8" max="8" width="12.875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1565,7 +1744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
@@ -1588,7 +1767,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
@@ -1612,7 +1791,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>64</v>
       </c>
@@ -1660,7 +1839,7 @@
       <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.875" style="12" customWidth="1"/>
     <col min="2" max="2" width="25.875" customWidth="1"/>
@@ -1671,7 +1850,7 @@
     <col min="7" max="7" width="12.875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1694,7 +1873,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
@@ -1712,7 +1891,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>41</v>
       </c>
@@ -1733,7 +1912,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>68</v>
       </c>
@@ -1741,28 +1920,28 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="13"/>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="13"/>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="13"/>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="13"/>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="13"/>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="13"/>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="13"/>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="13"/>
     </row>
   </sheetData>
@@ -1811,7 +1990,7 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.875" style="14" customWidth="1"/>
     <col min="2" max="2" width="25.875" customWidth="1"/>
@@ -1820,7 +1999,7 @@
     <col min="5" max="5" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="7" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:5" s="7" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1873,14 +2052,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="14.125" customWidth="1"/>
     <col min="3" max="3" width="16.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
@@ -1933,14 +2112,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.125" customWidth="1"/>
     <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>46</v>
       </c>
@@ -1957,7 +2136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
     </row>
@@ -2012,32 +2191,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="16" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:1" s="16" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2054,257 +2233,257 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.375" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75">
+    <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:1" ht="18.75">
+    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:1" ht="18.75">
+    <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:1" ht="18.75">
+    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:1" ht="18.75">
+    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:1" ht="18.75">
+    <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:1" ht="18.75">
+    <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:1" ht="18.75">
+    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:1" ht="18.75">
+    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:1" ht="18.75">
+    <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:1" ht="18.75">
+    <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:1" ht="18.75">
+    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:1" ht="18.75">
+    <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:1" ht="18.75">
+    <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:1" ht="18.75">
+    <row r="16" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" ht="18.75">
+    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" ht="18.75">
+    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" ht="18.75">
+    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" ht="18.75">
+    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" ht="18.75">
+    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" ht="18.75">
+    <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" ht="18.75">
+    <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" ht="18.75">
+    <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:1" ht="18.75">
+    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:1" ht="18.75">
+    <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:1" ht="18.75">
+    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:1" ht="18.75">
+    <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:1" ht="18.75">
+    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:1" ht="18.75">
+    <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:1" ht="18.75">
+    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:1" ht="18.75">
+    <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" ht="18.75">
+    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" ht="18.75">
+    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" ht="18.75">
+    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" ht="18.75">
+    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" ht="18.75">
+    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" ht="18.75">
+    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" ht="18.75">
+    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" ht="18.75">
+    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" ht="18.75">
+    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" ht="18.75">
+    <row r="42" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" ht="18.75">
+    <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" ht="18.75">
+    <row r="44" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" ht="18.75">
+    <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" ht="18.75">
+    <row r="46" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" ht="18.75">
+    <row r="47" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" ht="18.75">
+    <row r="48" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" ht="18.75">
+    <row r="49" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:1" ht="18.75">
+    <row r="50" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" ht="18.75">
+    <row r="51" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" ht="18.75">
+    <row r="52" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" ht="18.75">
+    <row r="53" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" ht="18.75">
+    <row r="54" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" ht="18.75">
+    <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" ht="18.75">
+    <row r="56" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" ht="18.75">
+    <row r="57" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" ht="18.75">
+    <row r="58" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" ht="18.75">
+    <row r="59" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" ht="18.75">
+    <row r="60" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" ht="18.75">
+    <row r="61" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" ht="18.75">
+    <row r="62" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1" ht="18.75">
+    <row r="63" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1" ht="18.75">
+    <row r="64" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" ht="18.75">
+    <row r="65" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" ht="18.75">
+    <row r="66" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" ht="18.75">
+    <row r="67" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" ht="18.75">
+    <row r="68" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" ht="18.75">
+    <row r="69" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" ht="18.75">
+    <row r="70" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" ht="18.75">
+    <row r="71" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" ht="18.75">
+    <row r="72" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:1" ht="18.75">
+    <row r="73" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:1" ht="18.75">
+    <row r="74" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:1" ht="18.75">
+    <row r="75" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:1" ht="18.75">
+    <row r="76" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:1" ht="18.75">
+    <row r="77" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1" ht="18.75">
+    <row r="78" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
     </row>
-    <row r="79" spans="1:1" ht="18.75">
+    <row r="79" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:1" ht="18.75">
+    <row r="80" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:1" ht="18.75">
+    <row r="81" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
     </row>
-    <row r="82" spans="1:1" ht="18.75">
+    <row r="82" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
     </row>
   </sheetData>
@@ -2351,12 +2530,12 @@
       <selection activeCell="B8" sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
@@ -2364,7 +2543,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>75</v>
       </c>
@@ -2372,7 +2551,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -2380,7 +2559,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -2388,7 +2567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2396,7 +2575,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2404,7 +2583,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>85</v>
       </c>
@@ -2412,7 +2591,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
added additional metadata, static csv columns for mapping and test option
adding static csv columns to input to support more mapping actions and including e.g. the conversion date to the ontology metadata

added test option to support automated basic testing by comparing the computed result ttl with an expected result
</commit_message>
<xml_diff>
--- a/test/test-input.xlsx
+++ b/test/test-input.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24BBF2A-910A-4437-AA45-9876AD897769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96307184-6920-43E8-8340-613DB815D9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,6 +49,7 @@
     <author>tc={E66E2A3F-7B19-4BB7-8DE0-C3E4C58A5B68}</author>
     <author>tc={8C82DEC2-E0DA-4628-BD35-89B1B0EC3B02}</author>
     <author>tc={E1ADD663-58B7-4105-8D38-8C3BDCFC6570}</author>
+    <author>tc={BEDAFE8F-06EA-4D62-A34A-2CCE447B0FD9}</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{6A6C5CF8-F4E8-4CA8-8374-C756CE1FDA5F}">
@@ -91,12 +92,20 @@
     dcterms:rights string to add to the ontology metadata</t>
       </text>
     </comment>
+    <comment ref="J1" authorId="5" shapeId="0" xr:uid="{BEDAFE8F-06EA-4D62-A34A-2CCE447B0FD9}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Last translation date, will get filled in by xlsx2owl script</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="105">
   <si>
     <t>Domain</t>
   </si>
@@ -408,6 +417,9 @@
   </si>
   <si>
     <t>Author 1;Author 2</t>
+  </si>
+  <si>
+    <t>xlsx2owl_datetime</t>
   </si>
 </sst>
 </file>
@@ -426,6 +438,7 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -433,6 +446,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -440,27 +454,32 @@
       <sz val="14"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -468,12 +487,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -495,7 +516,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1137,6 +1158,9 @@
   <threadedComment ref="H1" dT="2024-02-15T11:19:18.98" personId="{00000000-0000-0000-0000-000000000000}" id="{E1ADD663-58B7-4105-8D38-8C3BDCFC6570}">
     <text>dcterms:rights string to add to the ontology metadata</text>
   </threadedComment>
+  <threadedComment ref="J1" dT="2024-02-15T12:00:33.72" personId="{00000000-0000-0000-0000-000000000000}" id="{BEDAFE8F-06EA-4D62-A34A-2CCE447B0FD9}">
+    <text>Last translation date, will get filled in by xlsx2owl script</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1538,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1580,7 @@
     <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>54</v>
       </c>
@@ -1584,8 +1608,11 @@
       <c r="I1" s="29" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>

</xml_diff>